<commit_message>
Add Homeworks excel file
</commit_message>
<xml_diff>
--- a/Nelly_Harutyunyan_Homework_1.xlsx
+++ b/Nelly_Harutyunyan_Homework_1.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelly\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelly\Desktop\Git\Epam-session-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C071F3F-F9EC-475A-820D-10E9161A4FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7896404B-A671-4CF5-A374-C717C3A05518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug_Reporting" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Test_Scenario" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
   <si>
     <t>Bug ID</t>
   </si>
@@ -217,6 +217,42 @@
   </si>
   <si>
     <t>Bug_10</t>
+  </si>
+  <si>
+    <t>Test Scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check uploading of one PHS Request Document </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check uploading of multiple PHS Request Documents </t>
+  </si>
+  <si>
+    <t>Verify that documents are uploaded to the Documents section</t>
+  </si>
+  <si>
+    <t>Verify that documents with Other type are optional for the task could be submitted for approval</t>
+  </si>
+  <si>
+    <t>Verify that PHS Request Document can't be removed once it is approved</t>
+  </si>
+  <si>
+    <t>Verify documents with Other type can be removed after approving</t>
+  </si>
+  <si>
+    <t>Verify the right format is shown in Type field</t>
+  </si>
+  <si>
+    <t>Verify that at least one PHS Request Document should be uploaded before the task could be submitted for approval</t>
+  </si>
+  <si>
+    <t>Verify PHS Request Document can be removed before approving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check uploading of Other type of Document </t>
+  </si>
+  <si>
+    <t>Check uploading of multiple Other type of Documents</t>
   </si>
 </sst>
 </file>
@@ -226,7 +262,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,8 +293,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,8 +325,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -626,6 +674,17 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -634,26 +693,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -770,6 +814,45 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1054,9 +1137,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,304 +1155,304 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="7" t="s">
+      <c r="F1" s="45"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="14">
         <v>44325</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="40" t="s">
+      <c r="H3" s="35" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="18">
         <v>44325</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="36" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15">
+      <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="22">
         <v>44325</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="37" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="18">
         <v>44325</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="43" t="s">
+      <c r="H6" s="38" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15">
+      <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="22">
         <v>44325</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="39" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14">
+      <c r="A8" s="9">
         <v>6</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="18">
         <v>44325</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="36" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15">
+      <c r="A9" s="10">
         <v>7</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="22">
         <v>44325</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="42" t="s">
+      <c r="H9" s="37" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14">
+      <c r="A10" s="9">
         <v>8</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="18">
         <v>44325</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="41" t="s">
+      <c r="H10" s="36" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15">
+      <c r="A11" s="10">
         <v>9</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="22">
         <v>44325</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="42" t="s">
+      <c r="H11" s="37" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="70.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="16">
+      <c r="A12" s="11">
         <v>10</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="28">
         <v>44325</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="35" t="s">
+      <c r="G12" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="H12" s="45" t="s">
+      <c r="H12" s="40" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1397,12 +1480,115 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F753C5-BBAF-4A85-87E2-B09D3661FD1F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="97.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="47">
+        <v>1</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="48">
+        <v>2</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="47">
+        <v>3</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="48">
+        <v>4</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="47">
+        <v>5</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="48">
+        <v>6</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="47">
+        <v>7</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="48">
+        <v>8</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="47">
+        <v>9</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="48">
+        <v>10</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="49">
+        <v>11</v>
+      </c>
+      <c r="B12" s="53" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>